<commit_message>
update vergleich BM zu AB2
</commit_message>
<xml_diff>
--- a/doc/AB2 vs Berkeley Madonnaxlsx.xlsx
+++ b/doc/AB2 vs Berkeley Madonnaxlsx.xlsx
@@ -281,7 +281,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,13 +297,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -318,16 +332,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -346,15 +371,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kondensator table2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="intern_kondensator" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sim_kondensator2" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kondensator table2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29291,146 +29316,155 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:AC54"/>
+  <dimension ref="A1:AC54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="AB33" sqref="AB33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" customWidth="1"/>
     <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.42578125" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" style="4"/>
-    <col min="18" max="18" width="11.42578125" style="1"/>
+    <col min="18" max="18" width="11.42578125" style="6"/>
     <col min="19" max="20" width="5.140625" customWidth="1"/>
     <col min="21" max="24" width="12" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.5703125" customWidth="1"/>
+    <col min="27" max="27" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:29" ht="21">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+    <row r="1" spans="1:29" s="7" customFormat="1">
+      <c r="B1" s="8"/>
+      <c r="F1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="10"/>
+    </row>
+    <row r="2" spans="1:29" s="7" customFormat="1" ht="21">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="7" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="8"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5" t="s">
+      <c r="R2" s="14"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5" t="s">
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-    </row>
-    <row r="3" spans="1:29">
-      <c r="B3" s="3" t="s">
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+    </row>
+    <row r="3" spans="1:29" s="15" customFormat="1" ht="15.75">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AB3" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -29444,7 +29478,7 @@
       <c r="D4">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>9</v>
       </c>
       <c r="F4" s="4">
@@ -29459,7 +29493,7 @@
       <c r="J4">
         <v>1250</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="5">
         <v>9</v>
       </c>
       <c r="L4">
@@ -29478,7 +29512,7 @@
         <f>F4-M4</f>
         <v>0</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="6">
         <f>E4-K4</f>
         <v>0</v>
       </c>
@@ -29498,11 +29532,11 @@
         <v>7.7166415741750001</v>
       </c>
       <c r="Z4" s="4">
-        <f>F4-W4</f>
+        <f t="shared" ref="Z4:Z35" si="0">F4-W4</f>
         <v>-1.2833584258249999</v>
       </c>
-      <c r="AA4">
-        <f>E4-X4</f>
+      <c r="AA4" s="5">
+        <f t="shared" ref="AA4:AA35" si="1">E4-X4</f>
         <v>1.2833584258249999</v>
       </c>
       <c r="AB4">
@@ -29524,7 +29558,7 @@
       <c r="D5">
         <v>6.1733100000000004E-3</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>7.7166399999999999</v>
       </c>
       <c r="F5" s="4">
@@ -29539,7 +29573,7 @@
       <c r="J5">
         <v>1250</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="5">
         <v>7.7137010000000004</v>
       </c>
       <c r="L5">
@@ -29555,11 +29589,11 @@
         <v>6.1709599999999996E-3</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" ref="Q5:Q54" si="0">F5-M5</f>
+        <f t="shared" ref="Q5:Q54" si="2">F5-M5</f>
         <v>-2.9390000000000249E-3</v>
       </c>
-      <c r="R5" s="1">
-        <f t="shared" ref="R5:R54" si="1">E5-K5</f>
+      <c r="R5" s="6">
+        <f t="shared" ref="R5:R54" si="3">E5-K5</f>
         <v>2.9389999999995808E-3</v>
       </c>
       <c r="T5">
@@ -29578,19 +29612,19 @@
         <v>6.6162841315870002</v>
       </c>
       <c r="Z5" s="4">
-        <f>F5-W5</f>
+        <f t="shared" si="0"/>
         <v>-1.1003558684130001</v>
       </c>
-      <c r="AA5">
-        <f>E5-X5</f>
+      <c r="AA5" s="5">
+        <f t="shared" si="1"/>
         <v>1.1003558684129997</v>
       </c>
       <c r="AB5">
-        <f t="shared" ref="AB5:AB54" si="2">D5-U5</f>
+        <f t="shared" ref="AB5:AB54" si="4">D5-U5</f>
         <v>5.6442090050000003E-3</v>
       </c>
       <c r="AC5">
-        <f t="shared" ref="AC5:AC54" si="3">C5-V5</f>
+        <f t="shared" ref="AC5:AC54" si="5">C5-V5</f>
         <v>-5.721862520000001E-4</v>
       </c>
     </row>
@@ -29604,7 +29638,7 @@
       <c r="D6">
         <v>5.2930299999999998E-3</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>6.6162799999999997</v>
       </c>
       <c r="F6" s="4">
@@ -29619,7 +29653,7 @@
       <c r="J6">
         <v>1250</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="5">
         <v>6.6137620000000004</v>
       </c>
       <c r="L6">
@@ -29635,11 +29669,11 @@
         <v>5.2910099999999996E-3</v>
       </c>
       <c r="Q6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2.5180000000002423E-3</v>
       </c>
-      <c r="R6" s="1">
-        <f t="shared" si="1"/>
+      <c r="R6" s="6">
+        <f t="shared" si="3"/>
         <v>2.5179999999993541E-3</v>
       </c>
       <c r="T6">
@@ -29658,19 +29692,19 @@
         <v>5.6728325773729997</v>
       </c>
       <c r="Z6" s="4">
-        <f>F6-W6</f>
+        <f t="shared" si="0"/>
         <v>-0.94344742262699999</v>
       </c>
-      <c r="AA6">
-        <f>E6-X6</f>
+      <c r="AA6" s="5">
+        <f t="shared" si="1"/>
         <v>0.94344742262699999</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.8393763630000001E-3</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-4.9059705999999993E-4</v>
       </c>
     </row>
@@ -29684,7 +29718,7 @@
       <c r="D7">
         <v>4.5382699999999996E-3</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>5.6728300000000003</v>
       </c>
       <c r="F7" s="4">
@@ -29699,7 +29733,7 @@
       <c r="J7">
         <v>1250</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="5">
         <v>5.6706700000000003</v>
       </c>
       <c r="L7">
@@ -29715,11 +29749,11 @@
         <v>4.5365359999999999E-3</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2.1599999999999397E-3</v>
       </c>
-      <c r="R7" s="1">
-        <f t="shared" si="1"/>
+      <c r="R7" s="6">
+        <f t="shared" si="3"/>
         <v>2.1599999999999397E-3</v>
       </c>
       <c r="T7">
@@ -29738,19 +29772,19 @@
         <v>4.8639128566540002</v>
       </c>
       <c r="Z7" s="4">
-        <f>F7-W7</f>
+        <f t="shared" si="0"/>
         <v>-0.80891714334599962</v>
       </c>
-      <c r="AA7">
-        <f>E7-X7</f>
+      <c r="AA7" s="5">
+        <f t="shared" si="1"/>
         <v>0.80891714334600007</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.1493052759999996E-3</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-4.2063531499999976E-4</v>
       </c>
     </row>
@@ -29764,7 +29798,7 @@
       <c r="D8">
         <v>3.89113E-3</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>4.8639099999999997</v>
       </c>
       <c r="F8" s="4">
@@ -29779,7 +29813,7 @@
       <c r="J8">
         <v>1250</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="5">
         <v>4.8620590000000004</v>
       </c>
       <c r="L8">
@@ -29795,11 +29829,11 @@
         <v>3.889647E-3</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.8509999999993809E-3</v>
       </c>
-      <c r="R8" s="1">
-        <f t="shared" si="1"/>
+      <c r="R8" s="6">
+        <f t="shared" si="3"/>
         <v>1.8509999999993809E-3</v>
       </c>
       <c r="T8">
@@ -29818,19 +29852,19 @@
         <v>4.1703413514239998</v>
       </c>
       <c r="Z8" s="4">
-        <f>F8-W8</f>
+        <f t="shared" si="0"/>
         <v>-0.69356864857599998</v>
       </c>
-      <c r="AA8">
-        <f>E8-X8</f>
+      <c r="AA8" s="5">
+        <f t="shared" si="1"/>
         <v>0.69356864857599998</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.5576298490000002E-3</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.6065249699999968E-4</v>
       </c>
     </row>
@@ -29844,7 +29878,7 @@
       <c r="D9">
         <v>3.3362700000000001E-3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>4.1703400000000004</v>
       </c>
       <c r="F9" s="4">
@@ -29859,7 +29893,7 @@
       <c r="J9">
         <v>1250</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="5">
         <v>4.1687519999999996</v>
       </c>
       <c r="L9">
@@ -29875,11 +29909,11 @@
         <v>3.3350020000000001E-3</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.588000000000811E-3</v>
       </c>
-      <c r="R9" s="1">
-        <f t="shared" si="1"/>
+      <c r="R9" s="6">
+        <f t="shared" si="3"/>
         <v>1.588000000000811E-3</v>
       </c>
       <c r="T9">
@@ -29898,19 +29932,19 @@
         <v>3.5756699389889999</v>
       </c>
       <c r="Z9" s="4">
-        <f>F9-W9</f>
+        <f t="shared" si="0"/>
         <v>-0.59467006101100051</v>
       </c>
-      <c r="AA9">
-        <f>E9-X9</f>
+      <c r="AA9" s="5">
+        <f t="shared" si="1"/>
         <v>0.59467006101100051</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.05032543E-3</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.0923163200000017E-4</v>
       </c>
     </row>
@@ -29924,7 +29958,7 @@
       <c r="D10">
         <v>2.86054E-3</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>3.5756700000000001</v>
       </c>
       <c r="F10" s="4">
@@ -29939,7 +29973,7 @@
       <c r="J10">
         <v>1250</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="5">
         <v>3.5743070000000001</v>
       </c>
       <c r="L10">
@@ -29955,11 +29989,11 @@
         <v>2.8594459999999999E-3</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.362999999999559E-3</v>
       </c>
-      <c r="R10" s="1">
-        <f t="shared" si="1"/>
+      <c r="R10" s="6">
+        <f t="shared" si="3"/>
         <v>1.3630000000000031E-3</v>
       </c>
       <c r="T10">
@@ -29978,19 +30012,19 @@
         <v>3.06579592297</v>
       </c>
       <c r="Z10" s="4">
-        <f>F10-W10</f>
+        <f t="shared" si="0"/>
         <v>-0.50987407703000009</v>
       </c>
-      <c r="AA10">
-        <f>E10-X10</f>
+      <c r="AA10" s="5">
+        <f t="shared" si="1"/>
         <v>0.50987407703000009</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.615369804E-3</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2.6513611999999997E-4</v>
       </c>
     </row>
@@ -30004,7 +30038,7 @@
       <c r="D11">
         <v>2.4526399999999999E-3</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>3.0657999999999999</v>
       </c>
       <c r="F11" s="4">
@@ -30019,7 +30053,7 @@
       <c r="J11">
         <v>1250</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="5">
         <v>3.0646270000000002</v>
       </c>
       <c r="L11">
@@ -30035,11 +30069,11 @@
         <v>2.451702E-3</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.1730000000005347E-3</v>
       </c>
-      <c r="R11" s="1">
-        <f t="shared" si="1"/>
+      <c r="R11" s="6">
+        <f t="shared" si="3"/>
         <v>1.1729999999996465E-3</v>
       </c>
       <c r="T11">
@@ -30058,19 +30092,19 @@
         <v>2.6286275863470001</v>
       </c>
       <c r="Z11" s="4">
-        <f>F11-W11</f>
+        <f t="shared" si="0"/>
         <v>-0.43717241365300019</v>
       </c>
-      <c r="AA11">
-        <f>E11-X11</f>
+      <c r="AA11" s="5">
+        <f t="shared" si="1"/>
         <v>0.43717241365299975</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.2424299419999999E-3</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2.2732365499999975E-4</v>
       </c>
     </row>
@@ -30084,7 +30118,7 @@
       <c r="D12">
         <v>2.1029E-3</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>2.6286299999999998</v>
       </c>
       <c r="F12" s="4">
@@ -30099,7 +30133,7 @@
       <c r="J12">
         <v>1250</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="5">
         <v>2.6276259999999998</v>
       </c>
       <c r="L12">
@@ -30115,11 +30149,11 @@
         <v>2.1021009999999999E-3</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.0040000000000049E-3</v>
       </c>
-      <c r="R12" s="1">
-        <f t="shared" si="1"/>
+      <c r="R12" s="6">
+        <f t="shared" si="3"/>
         <v>1.0040000000000049E-3</v>
       </c>
       <c r="T12">
@@ -30138,19 +30172,19 @@
         <v>2.2537974350919998</v>
       </c>
       <c r="Z12" s="4">
-        <f>F12-W12</f>
+        <f t="shared" si="0"/>
         <v>-0.37483256490799999</v>
       </c>
-      <c r="AA12">
-        <f>E12-X12</f>
+      <c r="AA12" s="5">
+        <f t="shared" si="1"/>
         <v>0.37483256490799999</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9226649249999999E-3</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.949153339999999E-4</v>
       </c>
     </row>
@@ -30164,7 +30198,7 @@
       <c r="D13">
         <v>1.8030399999999999E-3</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <v>2.2538</v>
       </c>
       <c r="F13" s="4">
@@ -30179,7 +30213,7 @@
       <c r="J13">
         <v>1250</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="5">
         <v>2.2529379999999999</v>
       </c>
       <c r="L13">
@@ -30195,11 +30229,11 @@
         <v>1.802351E-3</v>
       </c>
       <c r="Q13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-8.6199999999969634E-4</v>
       </c>
-      <c r="R13" s="1">
-        <f t="shared" si="1"/>
+      <c r="R13" s="6">
+        <f t="shared" si="3"/>
         <v>8.6200000000014043E-4</v>
       </c>
       <c r="T13">
@@ -30218,19 +30252,19 @@
         <v>1.9324163319330001</v>
       </c>
       <c r="Z13" s="4">
-        <f>F13-W13</f>
+        <f t="shared" si="0"/>
         <v>-0.32138366806699992</v>
       </c>
-      <c r="AA13">
-        <f>E13-X13</f>
+      <c r="AA13" s="5">
+        <f t="shared" si="1"/>
         <v>0.32138366806699992</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.6485056139999999E-3</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.6711350700000013E-4</v>
       </c>
     </row>
@@ -30244,7 +30278,7 @@
       <c r="D14">
         <v>1.54593E-3</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="5">
         <v>1.93242</v>
       </c>
       <c r="F14" s="4">
@@ -30259,7 +30293,7 @@
       <c r="J14">
         <v>1250</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="5">
         <v>1.9316800000000001</v>
       </c>
       <c r="L14">
@@ -30275,11 +30309,11 @@
         <v>1.5453439999999999E-3</v>
       </c>
       <c r="Q14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-7.3999999999951882E-4</v>
       </c>
-      <c r="R14" s="1">
-        <f t="shared" si="1"/>
+      <c r="R14" s="6">
+        <f t="shared" si="3"/>
         <v>7.3999999999996291E-4</v>
       </c>
       <c r="T14">
@@ -30298,19 +30332,19 @@
         <v>1.656862689512</v>
       </c>
       <c r="Z14" s="4">
-        <f>F14-W14</f>
+        <f t="shared" si="0"/>
         <v>-0.27555731048799981</v>
       </c>
-      <c r="AA14">
-        <f>E14-X14</f>
+      <c r="AA14" s="5">
+        <f t="shared" si="1"/>
         <v>0.27555731048800003</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.4134315040000001E-3</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.4329140099999995E-4</v>
       </c>
     </row>
@@ -30324,7 +30358,7 @@
       <c r="D15">
         <v>1.3254899999999999E-3</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <v>1.65686</v>
       </c>
       <c r="F15" s="4">
@@ -30339,7 +30373,7 @@
       <c r="J15">
         <v>1250</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="5">
         <v>1.656231</v>
       </c>
       <c r="L15">
@@ -30355,11 +30389,11 @@
         <v>1.3249850000000001E-3</v>
       </c>
       <c r="Q15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-6.2899999999999068E-4</v>
       </c>
-      <c r="R15" s="1">
-        <f t="shared" si="1"/>
+      <c r="R15" s="6">
+        <f t="shared" si="3"/>
         <v>6.2899999999999068E-4</v>
       </c>
       <c r="T15">
@@ -30378,19 +30412,19 @@
         <v>1.420601723621</v>
       </c>
       <c r="Z15" s="4">
-        <f>F15-W15</f>
+        <f t="shared" si="0"/>
         <v>-0.23625827637899999</v>
       </c>
-      <c r="AA15">
-        <f>E15-X15</f>
+      <c r="AA15" s="5">
+        <f t="shared" si="1"/>
         <v>0.23625827637899999</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.2118851769999999E-3</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.2285710400000054E-4</v>
       </c>
     </row>
@@ -30404,7 +30438,7 @@
       <c r="D16">
         <v>1.13648E-3</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <v>1.4206000000000001</v>
       </c>
       <c r="F16" s="4">
@@ -30419,7 +30453,7 @@
       <c r="J16">
         <v>1250</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="5">
         <v>1.4200600000000001</v>
       </c>
       <c r="L16">
@@ -30435,11 +30469,11 @@
         <v>1.136048E-3</v>
       </c>
       <c r="Q16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-5.3999999999998494E-4</v>
       </c>
-      <c r="R16" s="1">
-        <f t="shared" si="1"/>
+      <c r="R16" s="6">
+        <f t="shared" si="3"/>
         <v>5.3999999999998494E-4</v>
       </c>
       <c r="T16">
@@ -30458,19 +30492,19 @@
         <v>1.218030480093</v>
       </c>
       <c r="Z16" s="4">
-        <f>F16-W16</f>
+        <f t="shared" si="0"/>
         <v>-0.20256951990700056</v>
       </c>
-      <c r="AA16">
-        <f>E16-X16</f>
+      <c r="AA16" s="5">
+        <f t="shared" si="1"/>
         <v>0.20256951990700012</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.0390747000000001E-3</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.0533414999999973E-4</v>
       </c>
     </row>
@@ -30484,7 +30518,7 @@
       <c r="D17" s="2">
         <v>9.7442399999999999E-4</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="5">
         <v>1.2180299999999999</v>
       </c>
       <c r="F17" s="4">
@@ -30499,7 +30533,7 @@
       <c r="J17">
         <v>1250</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="5">
         <v>1.2175659999999999</v>
       </c>
       <c r="L17">
@@ -30515,11 +30549,11 @@
         <v>9.7405300000000001E-4</v>
       </c>
       <c r="Q17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-4.6400000000001995E-4</v>
       </c>
-      <c r="R17" s="1">
-        <f t="shared" si="1"/>
+      <c r="R17" s="6">
+        <f t="shared" si="3"/>
         <v>4.6400000000001995E-4</v>
       </c>
       <c r="T17">
@@ -30538,19 +30572,19 @@
         <v>1.044344960144</v>
       </c>
       <c r="Z17" s="4">
-        <f>F17-W17</f>
+        <f t="shared" si="0"/>
         <v>-0.17368503985600015</v>
       </c>
-      <c r="AA17">
-        <f>E17-X17</f>
+      <c r="AA17" s="5">
+        <f t="shared" si="1"/>
         <v>0.17368503985599992</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.9090824600000004E-4</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-9.0320621000000191E-5</v>
       </c>
     </row>
@@ -30564,7 +30598,7 @@
       <c r="D18" s="2">
         <v>8.3547600000000004E-4</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="5">
         <v>1.04434</v>
       </c>
       <c r="F18" s="4">
@@ -30579,7 +30613,7 @@
       <c r="J18">
         <v>1250</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="5">
         <v>1.043947</v>
       </c>
       <c r="L18">
@@ -30595,11 +30629,11 @@
         <v>8.3515749999999995E-4</v>
       </c>
       <c r="Q18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-3.9299999999986568E-4</v>
       </c>
-      <c r="R18" s="1">
-        <f t="shared" si="1"/>
+      <c r="R18" s="6">
+        <f t="shared" si="3"/>
         <v>3.9300000000008772E-4</v>
       </c>
       <c r="T18">
@@ -30618,19 +30652,19 @@
         <v>0.89542619302500004</v>
       </c>
       <c r="Z18" s="4">
-        <f>F18-W18</f>
+        <f t="shared" si="0"/>
         <v>-0.1489138069750009</v>
       </c>
-      <c r="AA18">
-        <f>E18-X18</f>
+      <c r="AA18" s="5">
+        <f t="shared" si="1"/>
         <v>0.14891380697500001</v>
       </c>
       <c r="AB18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.6386920700000007E-4</v>
       </c>
       <c r="AC18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.7438379999999335E-5</v>
       </c>
     </row>
@@ -30644,7 +30678,7 @@
       <c r="D19" s="2">
         <v>7.16341E-4</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="5">
         <v>0.89542600000000006</v>
       </c>
       <c r="F19" s="4">
@@ -30659,7 +30693,7 @@
       <c r="J19">
         <v>1250</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="5">
         <v>0.89508489999999996</v>
       </c>
       <c r="L19">
@@ -30675,11 +30709,11 @@
         <v>7.1606790000000001E-4</v>
       </c>
       <c r="Q19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-3.4499999999937359E-4</v>
       </c>
-      <c r="R19" s="1">
-        <f t="shared" si="1"/>
+      <c r="R19" s="6">
+        <f t="shared" si="3"/>
         <v>3.4110000000009411E-4</v>
       </c>
       <c r="T19">
@@ -30698,19 +30732,19 @@
         <v>0.76774255418899995</v>
       </c>
       <c r="Z19" s="4">
-        <f>F19-W19</f>
+        <f t="shared" si="0"/>
         <v>-0.12768744581099867</v>
       </c>
-      <c r="AA19">
-        <f>E19-X19</f>
+      <c r="AA19" s="5">
+        <f t="shared" si="1"/>
         <v>0.12768344581100011</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.5494500499999996E-4</v>
       </c>
       <c r="AC19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-6.6393871999999646E-5</v>
       </c>
     </row>
@@ -30724,7 +30758,7 @@
       <c r="D20" s="2">
         <v>6.1419399999999998E-4</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="5">
         <v>0.76774299999999995</v>
       </c>
       <c r="F20" s="4">
@@ -30739,7 +30773,7 @@
       <c r="J20">
         <v>1250</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="5">
         <v>0.76744990000000002</v>
       </c>
       <c r="L20">
@@ -30755,11 +30789,11 @@
         <v>6.1395999999999998E-4</v>
       </c>
       <c r="Q20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2.899999999996794E-4</v>
       </c>
-      <c r="R20" s="1">
-        <f t="shared" si="1"/>
+      <c r="R20" s="6">
+        <f t="shared" si="3"/>
         <v>2.9309999999993508E-4</v>
       </c>
       <c r="T20">
@@ -30778,19 +30812,19 @@
         <v>0.65826601243600003</v>
       </c>
       <c r="Z20" s="4">
-        <f>F20-W20</f>
+        <f t="shared" si="0"/>
         <v>-0.10947398756399984</v>
       </c>
-      <c r="AA20">
-        <f>E20-X20</f>
+      <c r="AA20" s="5">
+        <f t="shared" si="1"/>
         <v>0.10947698756399993</v>
       </c>
       <c r="AB20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.6155278999999998E-4</v>
       </c>
       <c r="AC20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-5.6931674000000425E-5</v>
       </c>
     </row>
@@ -30804,7 +30838,7 @@
       <c r="D21" s="2">
         <v>5.2661299999999999E-4</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="5">
         <v>0.65826600000000002</v>
       </c>
       <c r="F21" s="4">
@@ -30819,7 +30853,7 @@
       <c r="J21">
         <v>1250</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="5">
         <v>0.65801509999999996</v>
       </c>
       <c r="L21">
@@ -30835,11 +30869,11 @@
         <v>5.2641210000000001E-4</v>
       </c>
       <c r="Q21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2.5499999999922807E-4</v>
       </c>
-      <c r="R21" s="1">
-        <f t="shared" si="1"/>
+      <c r="R21" s="6">
+        <f t="shared" si="3"/>
         <v>2.5090000000005386E-4</v>
       </c>
       <c r="T21">
@@ -30858,19 +30892,19 @@
         <v>0.56440031982500005</v>
       </c>
       <c r="Z21" s="4">
-        <f>F21-W21</f>
+        <f t="shared" si="0"/>
         <v>-9.3869680175000525E-2</v>
       </c>
-      <c r="AA21">
-        <f>E21-X21</f>
+      <c r="AA21" s="5">
+        <f t="shared" si="1"/>
         <v>9.3865680174999966E-2</v>
       </c>
       <c r="AB21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.81478183E-4</v>
       </c>
       <c r="AC21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-4.8811834000000304E-5</v>
       </c>
     </row>
@@ -30884,7 +30918,7 @@
       <c r="D22" s="2">
         <v>4.5152000000000001E-4</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="5">
         <v>0.56440000000000001</v>
       </c>
       <c r="F22" s="4">
@@ -30899,7 +30933,7 @@
       <c r="J22">
         <v>1250</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="5">
         <v>0.56418520000000005</v>
       </c>
       <c r="L22">
@@ -30915,10 +30949,10 @@
         <v>4.5134819999999998E-4</v>
       </c>
       <c r="Q22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2.1499999999896602E-4</v>
       </c>
-      <c r="R22" s="1">
+      <c r="R22" s="6">
         <f>E22-K22</f>
         <v>2.1479999999995947E-4</v>
       </c>
@@ -30938,19 +30972,19 @@
         <v>0.48391944138199999</v>
       </c>
       <c r="Z22" s="4">
-        <f>F22-W22</f>
+        <f t="shared" si="0"/>
         <v>-8.048055861799952E-2</v>
       </c>
-      <c r="AA22">
-        <f>E22-X22</f>
+      <c r="AA22" s="5">
+        <f t="shared" si="1"/>
         <v>8.048055861800002E-2</v>
       </c>
       <c r="AB22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.1282120000000002E-4</v>
       </c>
       <c r="AC22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-4.1851890000000648E-5</v>
       </c>
     </row>
@@ -30964,7 +30998,7 @@
       <c r="D23" s="2">
         <v>3.87136E-4</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="5">
         <v>0.48391899999999999</v>
       </c>
       <c r="F23" s="4">
@@ -30979,7 +31013,7 @@
       <c r="J23">
         <v>1250</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="5">
         <v>0.48373500000000003</v>
       </c>
       <c r="L23">
@@ -30995,11 +31029,11 @@
         <v>3.86988E-4</v>
       </c>
       <c r="Q23" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.8500000000010175E-4</v>
       </c>
-      <c r="R23" s="1">
-        <f t="shared" si="1"/>
+      <c r="R23" s="6">
+        <f t="shared" si="3"/>
         <v>1.8399999999996197E-4</v>
       </c>
       <c r="T23">
@@ -31018,19 +31052,19 @@
         <v>0.41491476443600001</v>
       </c>
       <c r="Z23" s="4">
-        <f>F23-W23</f>
+        <f t="shared" si="0"/>
         <v>-6.9005235563999179E-2</v>
       </c>
-      <c r="AA23">
-        <f>E23-X23</f>
+      <c r="AA23" s="5">
+        <f t="shared" si="1"/>
         <v>6.9004235563999983E-2</v>
       </c>
       <c r="AB23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.5395547E-4</v>
       </c>
       <c r="AC23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.5884321999999497E-5</v>
       </c>
     </row>
@@ -31044,7 +31078,7 @@
       <c r="D24" s="2">
         <v>3.3193200000000001E-4</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="5">
         <v>0.41491499999999998</v>
       </c>
       <c r="F24" s="4">
@@ -31059,7 +31093,7 @@
       <c r="J24">
         <v>1250</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="5">
         <v>0.41475659999999998</v>
       </c>
       <c r="L24">
@@ -31075,11 +31109,11 @@
         <v>3.3180530000000001E-4</v>
       </c>
       <c r="Q24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.6300000000057935E-4</v>
       </c>
-      <c r="R24" s="1">
-        <f t="shared" si="1"/>
+      <c r="R24" s="6">
+        <f t="shared" si="3"/>
         <v>1.5840000000000298E-4</v>
       </c>
       <c r="T24">
@@ -31098,19 +31132,19 @@
         <v>0.35574983566500001</v>
       </c>
       <c r="Z24" s="4">
-        <f>F24-W24</f>
+        <f t="shared" si="0"/>
         <v>-5.9170164335000663E-2</v>
       </c>
-      <c r="AA24">
-        <f>E24-X24</f>
+      <c r="AA24" s="5">
+        <f t="shared" si="1"/>
         <v>5.9165164334999965E-2</v>
       </c>
       <c r="AB24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.0348286000000003E-4</v>
       </c>
       <c r="AC24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.0770084999999503E-5</v>
       </c>
     </row>
@@ -31124,7 +31158,7 @@
       <c r="D25" s="2">
         <v>2.8459999999999998E-4</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="5">
         <v>0.35575000000000001</v>
       </c>
       <c r="F25" s="4">
@@ -31139,7 +31173,7 @@
       <c r="J25">
         <v>1250</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="5">
         <v>0.35561419999999999</v>
       </c>
       <c r="L25">
@@ -31155,11 +31189,11 @@
         <v>2.8449140000000003E-4</v>
       </c>
       <c r="Q25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.3600000000124624E-4</v>
       </c>
-      <c r="R25" s="1">
-        <f t="shared" si="1"/>
+      <c r="R25" s="6">
+        <f t="shared" si="3"/>
         <v>1.3580000000001924E-4</v>
       </c>
       <c r="T25">
@@ -31178,19 +31212,19 @@
         <v>0.305021552433</v>
       </c>
       <c r="Z25" s="4">
-        <f>F25-W25</f>
+        <f t="shared" si="0"/>
         <v>-5.072844756699979E-2</v>
       </c>
-      <c r="AA25">
-        <f>E25-X25</f>
+      <c r="AA25" s="5">
+        <f t="shared" si="1"/>
         <v>5.0728447567000012E-2</v>
       </c>
       <c r="AB25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.6020757599999996E-4</v>
       </c>
       <c r="AC25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2.6378793000000379E-5</v>
       </c>
     </row>
@@ -31204,7 +31238,7 @@
       <c r="D26" s="2">
         <v>2.4401699999999999E-4</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="5">
         <v>0.30502200000000002</v>
       </c>
       <c r="F26" s="4">
@@ -31219,7 +31253,7 @@
       <c r="J26">
         <v>1250</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="5">
         <v>0.30490529999999999</v>
       </c>
       <c r="L26">
@@ -31235,11 +31269,11 @@
         <v>2.439242E-4</v>
       </c>
       <c r="Q26" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.1500000000097543E-4</v>
       </c>
-      <c r="R26" s="1">
-        <f t="shared" si="1"/>
+      <c r="R26" s="6">
+        <f t="shared" si="3"/>
         <v>1.1670000000002512E-4</v>
       </c>
       <c r="T26">
@@ -31258,19 +31292,19 @@
         <v>0.26152688805800001</v>
       </c>
       <c r="Z26" s="4">
-        <f>F26-W26</f>
+        <f t="shared" si="0"/>
         <v>-4.349311194200034E-2</v>
       </c>
-      <c r="AA26">
-        <f>E26-X26</f>
+      <c r="AA26" s="5">
+        <f t="shared" si="1"/>
         <v>4.3495111942000009E-2</v>
       </c>
       <c r="AB26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.23102823E-4</v>
       </c>
       <c r="AC26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2.2616017999999537E-5</v>
       </c>
     </row>
@@ -31284,7 +31318,7 @@
       <c r="D27" s="2">
         <v>2.0922200000000001E-4</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="5">
         <v>0.26152700000000001</v>
       </c>
       <c r="F27" s="4">
@@ -31299,7 +31333,7 @@
       <c r="J27">
         <v>1250</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="5">
         <v>0.26142720000000003</v>
       </c>
       <c r="L27">
@@ -31315,11 +31349,11 @@
         <v>2.0914180000000001E-4</v>
       </c>
       <c r="Q27" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.0300000000107445E-4</v>
       </c>
-      <c r="R27" s="1">
-        <f t="shared" si="1"/>
+      <c r="R27" s="6">
+        <f t="shared" si="3"/>
         <v>9.9799999999983235E-5</v>
       </c>
       <c r="T27">
@@ -31338,19 +31372,19 @@
         <v>0.22423436190599999</v>
       </c>
       <c r="Z27" s="4">
-        <f>F27-W27</f>
+        <f t="shared" si="0"/>
         <v>-3.7295638094001049E-2</v>
       </c>
-      <c r="AA27">
-        <f>E27-X27</f>
+      <c r="AA27" s="5">
+        <f t="shared" si="1"/>
         <v>3.7292638094000019E-2</v>
       </c>
       <c r="AB27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9129008800000002E-4</v>
       </c>
       <c r="AC27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.9388131999999864E-5</v>
       </c>
     </row>
@@ -31364,7 +31398,7 @@
       <c r="D28" s="2">
         <v>1.7938700000000001E-4</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="5">
         <v>0.22423399999999999</v>
       </c>
       <c r="F28" s="4">
@@ -31379,7 +31413,7 @@
       <c r="J28">
         <v>1250</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="5">
         <v>0.22414890000000001</v>
       </c>
       <c r="L28">
@@ -31395,11 +31429,11 @@
         <v>1.793191E-4</v>
       </c>
       <c r="Q28" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-8.0999999999775696E-5</v>
       </c>
-      <c r="R28" s="1">
-        <f t="shared" si="1"/>
+      <c r="R28" s="6">
+        <f t="shared" si="3"/>
         <v>8.5099999999976861E-5</v>
       </c>
       <c r="T28">
@@ -31418,19 +31452,19 @@
         <v>0.192259577716</v>
       </c>
       <c r="Z28" s="4">
-        <f>F28-W28</f>
+        <f t="shared" si="0"/>
         <v>-3.1970422284000932E-2</v>
       </c>
-      <c r="AA28">
-        <f>E28-X28</f>
+      <c r="AA28" s="5">
+        <f t="shared" si="1"/>
         <v>3.1974422283999993E-2</v>
       </c>
       <c r="AB28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.64012096E-4</v>
       </c>
       <c r="AC28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.6625020000000067E-5</v>
       </c>
     </row>
@@ -31444,7 +31478,7 @@
       <c r="D29" s="2">
         <v>1.5380799999999999E-4</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="5">
         <v>0.19225999999999999</v>
       </c>
       <c r="F29" s="4">
@@ -31459,7 +31493,7 @@
       <c r="J29">
         <v>1250</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="5">
         <v>0.1921863</v>
       </c>
       <c r="L29">
@@ -31475,11 +31509,11 @@
         <v>1.5374900000000001E-4</v>
       </c>
       <c r="Q29" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-7.3999999999685429E-5</v>
       </c>
-      <c r="R29" s="1">
-        <f t="shared" si="1"/>
+      <c r="R29" s="6">
+        <f t="shared" si="3"/>
         <v>7.3699999999982113E-5</v>
       </c>
       <c r="T29">
@@ -31498,19 +31532,19 @@
         <v>0.16484425004799999</v>
       </c>
       <c r="Z29" s="4">
-        <f>F29-W29</f>
+        <f t="shared" si="0"/>
         <v>-2.7415749951998691E-2</v>
       </c>
-      <c r="AA29">
-        <f>E29-X29</f>
+      <c r="AA29" s="5">
+        <f t="shared" si="1"/>
         <v>2.7415749951999996E-2</v>
       </c>
       <c r="AB29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.40625486E-4</v>
       </c>
       <c r="AC29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.4250989999999887E-5</v>
       </c>
     </row>
@@ -31524,7 +31558,7 @@
       <c r="D30" s="2">
         <v>1.3187499999999999E-4</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="5">
         <v>0.16484399999999999</v>
       </c>
       <c r="F30" s="4">
@@ -31539,7 +31573,7 @@
       <c r="J30">
         <v>1250</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="5">
         <v>0.16478139999999999</v>
       </c>
       <c r="L30">
@@ -31555,11 +31589,11 @@
         <v>1.318251E-4</v>
       </c>
       <c r="Q30" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-5.9000000000253294E-5</v>
       </c>
-      <c r="R30" s="1">
-        <f t="shared" si="1"/>
+      <c r="R30" s="6">
+        <f t="shared" si="3"/>
         <v>6.2599999999995992E-5</v>
       </c>
       <c r="T30">
@@ -31578,19 +31612,19 @@
         <v>0.141338221465</v>
       </c>
       <c r="Z30" s="4">
-        <f>F30-W30</f>
+        <f t="shared" si="0"/>
         <v>-2.3501778534999573E-2</v>
       </c>
-      <c r="AA30">
-        <f>E30-X30</f>
+      <c r="AA30" s="5">
+        <f t="shared" si="1"/>
         <v>2.3505778534999994E-2</v>
       </c>
       <c r="AB30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.2057225199999999E-4</v>
       </c>
       <c r="AC30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.222412499999985E-5</v>
       </c>
     </row>
@@ -31604,7 +31638,7 @@
       <c r="D31" s="2">
         <v>1.13071E-4</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="5">
         <v>0.14133799999999999</v>
       </c>
       <c r="F31" s="4">
@@ -31619,7 +31653,7 @@
       <c r="J31">
         <v>1250</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="5">
         <v>0.1412844</v>
       </c>
       <c r="L31">
@@ -31635,11 +31669,11 @@
         <v>1.1302749999999999E-4</v>
       </c>
       <c r="Q31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-5.5999999998945782E-5</v>
       </c>
-      <c r="R31" s="1">
-        <f t="shared" si="1"/>
+      <c r="R31" s="6">
+        <f t="shared" si="3"/>
         <v>5.3599999999986991E-5</v>
       </c>
       <c r="T31">
@@ -31658,19 +31692,19 @@
         <v>0.121184043975</v>
       </c>
       <c r="Z31" s="4">
-        <f>F31-W31</f>
+        <f t="shared" si="0"/>
         <v>-2.0155956025000421E-2</v>
       </c>
-      <c r="AA31">
-        <f>E31-X31</f>
+      <c r="AA31" s="5">
+        <f t="shared" si="1"/>
         <v>2.0153956024999989E-2</v>
       </c>
       <c r="AB31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.03379971E-4</v>
       </c>
       <c r="AC31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.0484296999999955E-5</v>
       </c>
     </row>
@@ -31684,7 +31718,7 @@
       <c r="D32" s="2">
         <v>9.6947200000000006E-5</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="5">
         <v>0.121184</v>
       </c>
       <c r="F32" s="4">
@@ -31699,7 +31733,7 @@
       <c r="J32">
         <v>1250</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="5">
         <v>0.12113790000000001</v>
       </c>
       <c r="L32">
@@ -31715,11 +31749,11 @@
         <v>9.6910289999999999E-5</v>
       </c>
       <c r="Q32" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-4.2000000000541604E-5</v>
       </c>
-      <c r="R32" s="1">
-        <f t="shared" si="1"/>
+      <c r="R32" s="6">
+        <f t="shared" si="3"/>
         <v>4.6099999999993369E-5</v>
       </c>
       <c r="T32">
@@ -31738,19 +31772,19 @@
         <v>0.103903759096</v>
       </c>
       <c r="Z32" s="4">
-        <f>F32-W32</f>
+        <f t="shared" si="0"/>
         <v>-1.7276240904001483E-2</v>
       </c>
-      <c r="AA32">
-        <f>E32-X32</f>
+      <c r="AA32" s="5">
+        <f t="shared" si="1"/>
         <v>1.7280240904000002E-2</v>
       </c>
       <c r="AB32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.8638067000000004E-5</v>
       </c>
       <c r="AC32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-8.9900450000006404E-6</v>
       </c>
     </row>
@@ -31764,7 +31798,7 @@
       <c r="D33" s="2">
         <v>8.3122999999999997E-5</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="5">
         <v>0.103904</v>
       </c>
       <c r="F33" s="4">
@@ -31779,7 +31813,7 @@
       <c r="J33">
         <v>1250</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="5">
         <v>0.1038642</v>
       </c>
       <c r="L33">
@@ -31795,11 +31829,11 @@
         <v>8.3091330000000004E-5</v>
       </c>
       <c r="Q33" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-3.5999999999702936E-5</v>
       </c>
-      <c r="R33" s="1">
-        <f t="shared" si="1"/>
+      <c r="R33" s="6">
+        <f t="shared" si="3"/>
         <v>3.9799999999992619E-5</v>
       </c>
       <c r="T33">
@@ -31818,19 +31852,19 @@
         <v>8.9087563016999993E-2</v>
       </c>
       <c r="Z33" s="4">
-        <f>F33-W33</f>
+        <f t="shared" si="0"/>
         <v>-1.4812436983000055E-2</v>
       </c>
-      <c r="AA33">
-        <f>E33-X33</f>
+      <c r="AA33" s="5">
+        <f t="shared" si="1"/>
         <v>1.4816436983000003E-2</v>
       </c>
       <c r="AB33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.5998710999999991E-5</v>
       </c>
       <c r="AC33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.704467000000173E-6</v>
       </c>
     </row>
@@ -31844,7 +31878,7 @@
       <c r="D34" s="2">
         <v>7.127E-5</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="5">
         <v>8.9087600000000003E-2</v>
       </c>
       <c r="F34" s="4">
@@ -31859,7 +31893,7 @@
       <c r="J34">
         <v>1250</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="5">
         <v>8.9053610000000005E-2</v>
       </c>
       <c r="L34">
@@ -31875,11 +31909,11 @@
         <v>7.1242890000000001E-5</v>
       </c>
       <c r="Q34" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-3.5999999999702936E-5</v>
       </c>
-      <c r="R34" s="1">
-        <f t="shared" si="1"/>
+      <c r="R34" s="6">
+        <f t="shared" si="3"/>
         <v>3.3989999999997633E-5</v>
       </c>
       <c r="T34">
@@ -31898,19 +31932,19 @@
         <v>7.6384088057999996E-2</v>
       </c>
       <c r="Z34" s="4">
-        <f>F34-W34</f>
+        <f t="shared" si="0"/>
         <v>-1.2705911942001435E-2</v>
       </c>
-      <c r="AA34">
-        <f>E34-X34</f>
+      <c r="AA34" s="5">
+        <f t="shared" si="1"/>
         <v>1.2703511942000006E-2</v>
       </c>
       <c r="AB34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.5161602000000002E-5</v>
       </c>
       <c r="AC34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-6.6102739999995483E-6</v>
       </c>
     </row>
@@ -31924,7 +31958,7 @@
       <c r="D35" s="2">
         <v>6.1107300000000004E-5</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="5">
         <v>7.6384099999999996E-2</v>
       </c>
       <c r="F35" s="4">
@@ -31939,7 +31973,7 @@
       <c r="J35">
         <v>1250</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="5">
         <v>7.6354980000000003E-2</v>
       </c>
       <c r="L35">
@@ -31955,11 +31989,11 @@
         <v>6.1083979999999999E-5</v>
       </c>
       <c r="Q35" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2.5000000000829914E-5</v>
       </c>
-      <c r="R35" s="1">
-        <f t="shared" si="1"/>
+      <c r="R35" s="6">
+        <f t="shared" si="3"/>
         <v>2.9119999999993595E-5</v>
       </c>
       <c r="T35">
@@ -31978,19 +32012,19 @@
         <v>6.5492069946000001E-2</v>
       </c>
       <c r="Z35" s="4">
-        <f>F35-W35</f>
+        <f t="shared" si="0"/>
         <v>-1.088793005400035E-2</v>
       </c>
-      <c r="AA35">
-        <f>E35-X35</f>
+      <c r="AA35" s="5">
+        <f t="shared" si="1"/>
         <v>1.0892030053999996E-2</v>
       </c>
       <c r="AB35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.5869931000000003E-5</v>
       </c>
       <c r="AC35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-5.6641240000002147E-6</v>
       </c>
     </row>
@@ -32004,7 +32038,7 @@
       <c r="D36" s="2">
         <v>5.2393699999999999E-5</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="5">
         <v>6.5492099999999998E-2</v>
       </c>
       <c r="F36" s="4">
@@ -32019,7 +32053,7 @@
       <c r="J36">
         <v>1250</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="5">
         <v>6.5467109999999995E-2</v>
       </c>
       <c r="L36">
@@ -32035,11 +32069,11 @@
         <v>5.2373690000000002E-5</v>
       </c>
       <c r="Q36" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2.3000000000550358E-5</v>
       </c>
-      <c r="R36" s="1">
-        <f t="shared" si="1"/>
+      <c r="R36" s="6">
+        <f t="shared" si="3"/>
         <v>2.499000000000251E-5</v>
       </c>
       <c r="T36">
@@ -32058,19 +32092,19 @@
         <v>5.6153203302999999E-2</v>
       </c>
       <c r="Z36" s="4">
-        <f>F36-W36</f>
+        <f t="shared" ref="Z36:Z54" si="6">F36-W36</f>
         <v>-9.3367966970010485E-3</v>
       </c>
-      <c r="AA36">
-        <f>E36-X36</f>
+      <c r="AA36" s="5">
+        <f t="shared" ref="AA36:AA54" si="7">E36-X36</f>
         <v>9.3388966969999987E-3</v>
       </c>
       <c r="AB36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.7903155999999999E-5</v>
       </c>
       <c r="AC36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-4.8603339999992931E-6</v>
       </c>
     </row>
@@ -32084,7 +32118,7 @@
       <c r="D37" s="2">
         <v>4.4922600000000003E-5</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="5">
         <v>5.61532E-2</v>
       </c>
       <c r="F37" s="4">
@@ -32099,7 +32133,7 @@
       <c r="J37">
         <v>1250</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="5">
         <v>5.6131800000000003E-2</v>
       </c>
       <c r="L37">
@@ -32115,11 +32149,11 @@
         <v>4.4905440000000001E-5</v>
       </c>
       <c r="Q37" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.8000000000739647E-5</v>
       </c>
-      <c r="R37" s="1">
-        <f t="shared" si="1"/>
+      <c r="R37" s="6">
+        <f t="shared" si="3"/>
         <v>2.139999999999781E-5</v>
       </c>
       <c r="T37">
@@ -32138,19 +32172,19 @@
         <v>4.8146015903000002E-2</v>
       </c>
       <c r="Z37" s="4">
-        <f>F37-W37</f>
+        <f t="shared" si="6"/>
         <v>-8.0039840969998721E-3</v>
       </c>
-      <c r="AA37">
-        <f>E37-X37</f>
+      <c r="AA37" s="5">
+        <f t="shared" si="7"/>
         <v>8.0071840969999988E-3</v>
       </c>
       <c r="AB37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.1072387000000001E-5</v>
       </c>
       <c r="AC37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-4.1640719999997897E-6</v>
       </c>
     </row>
@@ -32164,7 +32198,7 @@
       <c r="D38" s="2">
         <v>3.8516799999999997E-5</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="5">
         <v>4.8146000000000001E-2</v>
       </c>
       <c r="F38" s="4">
@@ -32179,7 +32213,7 @@
       <c r="J38">
         <v>1250</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="5">
         <v>4.8127669999999997E-2</v>
       </c>
       <c r="L38">
@@ -32195,11 +32229,11 @@
         <v>3.8502130000000001E-5</v>
       </c>
       <c r="Q38" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2.1999999999522402E-5</v>
       </c>
-      <c r="R38" s="1">
-        <f t="shared" si="1"/>
+      <c r="R38" s="6">
+        <f t="shared" si="3"/>
         <v>1.8330000000003899E-5</v>
       </c>
       <c r="T38">
@@ -32218,19 +32252,19 @@
         <v>4.1280616439000002E-2</v>
       </c>
       <c r="Z38" s="4">
-        <f>F38-W38</f>
+        <f t="shared" si="6"/>
         <v>-6.8693835609998644E-3</v>
       </c>
-      <c r="AA38">
-        <f>E38-X38</f>
+      <c r="AA38" s="5">
+        <f t="shared" si="7"/>
         <v>6.8653835609999991E-3</v>
       </c>
       <c r="AB38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.5215609E-5</v>
       </c>
       <c r="AC38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.5740790000002298E-6</v>
       </c>
     </row>
@@ -32244,7 +32278,7 @@
       <c r="D39" s="2">
         <v>3.3024500000000002E-5</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="5">
         <v>4.1280600000000001E-2</v>
       </c>
       <c r="F39" s="4">
@@ -32259,7 +32293,7 @@
       <c r="J39">
         <v>1250</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="5">
         <v>4.1264879999999997E-2</v>
       </c>
       <c r="L39">
@@ -32275,11 +32309,11 @@
         <v>3.3011910000000002E-5</v>
       </c>
       <c r="Q39" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.5000000001208491E-5</v>
       </c>
-      <c r="R39" s="1">
-        <f t="shared" si="1"/>
+      <c r="R39" s="6">
+        <f t="shared" si="3"/>
         <v>1.5720000000003787E-5</v>
       </c>
       <c r="T39">
@@ -32298,19 +32332,19 @@
         <v>3.5394191223999998E-2</v>
       </c>
       <c r="Z39" s="4">
-        <f>F39-W39</f>
+        <f t="shared" si="6"/>
         <v>-5.8858087760000899E-3</v>
       </c>
-      <c r="AA39">
-        <f>E39-X39</f>
+      <c r="AA39" s="5">
+        <f t="shared" si="7"/>
         <v>5.8864087760000031E-3</v>
       </c>
       <c r="AB39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.0194044000000003E-5</v>
       </c>
       <c r="AC39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.0650209999994946E-6</v>
       </c>
     </row>
@@ -32324,7 +32358,7 @@
       <c r="D40" s="2">
         <v>2.83154E-5</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="5">
         <v>3.5394200000000001E-2</v>
       </c>
       <c r="F40" s="4">
@@ -32339,7 +32373,7 @@
       <c r="J40">
         <v>1250</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="5">
         <v>3.5380700000000001E-2</v>
       </c>
       <c r="L40">
@@ -32355,11 +32389,11 @@
         <v>2.8304560000000001E-5</v>
       </c>
       <c r="Q40" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-9.0000000003698233E-6</v>
       </c>
-      <c r="R40" s="1">
-        <f t="shared" si="1"/>
+      <c r="R40" s="6">
+        <f t="shared" si="3"/>
         <v>1.3499999999999623E-5</v>
       </c>
       <c r="T40">
@@ -32378,19 +32412,19 @@
         <v>3.0347143053999999E-2</v>
       </c>
       <c r="Z40" s="4">
-        <f>F40-W40</f>
+        <f t="shared" si="6"/>
         <v>-5.0428569459999295E-3</v>
       </c>
-      <c r="AA40">
-        <f>E40-X40</f>
+      <c r="AA40" s="5">
+        <f t="shared" si="7"/>
         <v>5.0470569460000017E-3</v>
       </c>
       <c r="AB40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5888553999999999E-5</v>
       </c>
       <c r="AC40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2.6294859999994452E-6</v>
       </c>
     </row>
@@ -32404,7 +32438,7 @@
       <c r="D41" s="2">
         <v>2.42777E-5</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="5">
         <v>3.0347099999999998E-2</v>
       </c>
       <c r="F41" s="4">
@@ -32419,7 +32453,7 @@
       <c r="J41">
         <v>1250</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="5">
         <v>3.0335580000000001E-2</v>
       </c>
       <c r="L41">
@@ -32435,11 +32469,11 @@
         <v>2.426846E-5</v>
       </c>
       <c r="Q41" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.4000000000180535E-5</v>
       </c>
-      <c r="R41" s="1">
-        <f t="shared" si="1"/>
+      <c r="R41" s="6">
+        <f t="shared" si="3"/>
         <v>1.1519999999997504E-5</v>
       </c>
       <c r="T41">
@@ -32458,19 +32492,19 @@
         <v>2.6019780639000002E-2</v>
       </c>
       <c r="Z41" s="4">
-        <f>F41-W41</f>
+        <f t="shared" si="6"/>
         <v>-4.3302193609999762E-3</v>
       </c>
-      <c r="AA41">
-        <f>E41-X41</f>
+      <c r="AA41" s="5">
+        <f t="shared" si="7"/>
         <v>4.3273193609999969E-3</v>
       </c>
       <c r="AB41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.2196911000000001E-5</v>
       </c>
       <c r="AC41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2.2497139999999236E-6</v>
       </c>
     </row>
@@ -32484,7 +32518,7 @@
       <c r="D42" s="2">
         <v>2.0815800000000002E-5</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="5">
         <v>2.6019799999999999E-2</v>
       </c>
       <c r="F42" s="4">
@@ -32499,7 +32533,7 @@
       <c r="J42">
         <v>1250</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="5">
         <v>2.6009859999999999E-2</v>
       </c>
       <c r="L42">
@@ -32515,11 +32549,11 @@
         <v>2.080789E-5</v>
       </c>
       <c r="Q42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.000000000139778E-5</v>
       </c>
-      <c r="R42" s="1">
-        <f t="shared" si="1"/>
+      <c r="R42" s="6">
+        <f t="shared" si="3"/>
         <v>9.9399999999999489E-6</v>
       </c>
       <c r="T42">
@@ -32538,19 +32572,19 @@
         <v>2.2309480114E-2</v>
       </c>
       <c r="Z42" s="4">
-        <f>F42-W42</f>
+        <f t="shared" si="6"/>
         <v>-3.710519886000796E-3</v>
       </c>
-      <c r="AA42">
-        <f>E42-X42</f>
+      <c r="AA42" s="5">
+        <f t="shared" si="7"/>
         <v>3.7103198859999992E-3</v>
       </c>
       <c r="AB42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9031722000000003E-5</v>
       </c>
       <c r="AC42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.9290700000000605E-6</v>
       </c>
     </row>
@@ -32564,7 +32598,7 @@
       <c r="D43" s="2">
         <v>1.7847599999999998E-5</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="5">
         <v>2.2309499999999999E-2</v>
       </c>
       <c r="F43" s="4">
@@ -32579,7 +32613,7 @@
       <c r="J43">
         <v>1250</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="5">
         <v>2.2300980000000001E-2</v>
       </c>
       <c r="L43">
@@ -32595,11 +32629,11 @@
         <v>1.7840779999999999E-5</v>
       </c>
       <c r="Q43" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-8.9999999985934664E-6</v>
       </c>
-      <c r="R43" s="1">
-        <f t="shared" si="1"/>
+      <c r="R43" s="6">
+        <f t="shared" si="3"/>
         <v>8.5199999999979736E-6</v>
       </c>
       <c r="T43">
@@ -32618,19 +32652,19 @@
         <v>1.9128251305E-2</v>
       </c>
       <c r="Z43" s="4">
-        <f>F43-W43</f>
+        <f t="shared" si="6"/>
         <v>-3.181748694998987E-3</v>
       </c>
-      <c r="AA43">
-        <f>E43-X43</f>
+      <c r="AA43" s="5">
+        <f t="shared" si="7"/>
         <v>3.1812486949999996E-3</v>
       </c>
       <c r="AB43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.6317922999999998E-5</v>
       </c>
       <c r="AC43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.6533089999999639E-6</v>
       </c>
     </row>
@@ -32644,7 +32678,7 @@
       <c r="D44" s="2">
         <v>1.5302600000000002E-5</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="5">
         <v>1.9128300000000001E-2</v>
       </c>
       <c r="F44" s="4">
@@ -32659,7 +32693,7 @@
       <c r="J44">
         <v>1250</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="5">
         <v>1.9120959999999999E-2</v>
       </c>
       <c r="L44">
@@ -32675,11 +32709,11 @@
         <v>1.529677E-5</v>
       </c>
       <c r="Q44" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-9.0000000003698233E-6</v>
       </c>
-      <c r="R44" s="1">
-        <f t="shared" si="1"/>
+      <c r="R44" s="6">
+        <f t="shared" si="3"/>
         <v>7.340000000001512E-6</v>
       </c>
       <c r="T44">
@@ -32698,19 +32732,19 @@
         <v>1.6400651028999999E-2</v>
       </c>
       <c r="Z44" s="4">
-        <f>F44-W44</f>
+        <f t="shared" si="6"/>
         <v>-2.7293489710000784E-3</v>
       </c>
-      <c r="AA44">
-        <f>E44-X44</f>
+      <c r="AA44" s="5">
+        <f t="shared" si="7"/>
         <v>2.7276489710000018E-3</v>
       </c>
       <c r="AB44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.3991048000000002E-5</v>
       </c>
       <c r="AC44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.4216610000001087E-6</v>
       </c>
     </row>
@@ -32724,7 +32758,7 @@
       <c r="D45" s="2">
         <v>1.3120500000000001E-5</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="5">
         <v>1.6400700000000001E-2</v>
       </c>
       <c r="F45" s="4">
@@ -32739,7 +32773,7 @@
       <c r="J45">
         <v>1250</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="5">
         <v>1.63944E-2</v>
       </c>
       <c r="L45">
@@ -32755,11 +32789,11 @@
         <v>1.311552E-5</v>
       </c>
       <c r="Q45" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-6.0000000008386678E-6</v>
       </c>
-      <c r="R45" s="1">
-        <f t="shared" si="1"/>
+      <c r="R45" s="6">
+        <f t="shared" si="3"/>
         <v>6.3000000000007494E-6</v>
       </c>
       <c r="T45">
@@ -32778,19 +32812,19 @@
         <v>1.4061993953E-2</v>
       </c>
       <c r="Z45" s="4">
-        <f>F45-W45</f>
+        <f t="shared" si="6"/>
         <v>-2.3380060470010733E-3</v>
       </c>
-      <c r="AA45">
-        <f>E45-X45</f>
+      <c r="AA45" s="5">
+        <f t="shared" si="7"/>
         <v>2.3387060470000005E-3</v>
       </c>
       <c r="AB45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.1995969E-5</v>
       </c>
       <c r="AC45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.2177630000003922E-6</v>
       </c>
     </row>
@@ -32804,7 +32838,7 @@
       <c r="D46" s="2">
         <v>1.12496E-5</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="5">
         <v>1.4062E-2</v>
       </c>
       <c r="F46" s="4">
@@ -32819,7 +32853,7 @@
       <c r="J46">
         <v>1250</v>
       </c>
-      <c r="K46">
+      <c r="K46" s="5">
         <v>1.4056630000000001E-2</v>
       </c>
       <c r="L46">
@@ -32835,11 +32869,11 @@
         <v>1.124531E-5</v>
       </c>
       <c r="Q46" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-3.0000000013075123E-6</v>
       </c>
-      <c r="R46" s="1">
-        <f t="shared" si="1"/>
+      <c r="R46" s="6">
+        <f t="shared" si="3"/>
         <v>5.3699999999993336E-6</v>
       </c>
       <c r="T46">
@@ -32858,19 +32892,19 @@
         <v>1.2056818572E-2</v>
       </c>
       <c r="Z46" s="4">
-        <f>F46-W46</f>
+        <f t="shared" si="6"/>
         <v>-2.0031814279999338E-3</v>
       </c>
-      <c r="AA46">
-        <f>E46-X46</f>
+      <c r="AA46" s="5">
+        <f t="shared" si="7"/>
         <v>2.005181428E-3</v>
       </c>
       <c r="AB46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.0285422E-5</v>
       </c>
       <c r="AC46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.0404539999998158E-6</v>
       </c>
     </row>
@@ -32884,7 +32918,7 @@
       <c r="D47" s="2">
         <v>9.64546E-6</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="5">
         <v>1.2056799999999999E-2</v>
       </c>
       <c r="F47" s="4">
@@ -32899,7 +32933,7 @@
       <c r="J47">
         <v>1250</v>
       </c>
-      <c r="K47">
+      <c r="K47" s="5">
         <v>1.2052220000000001E-2</v>
       </c>
       <c r="L47">
@@ -32915,11 +32949,11 @@
         <v>9.6417790000000006E-6</v>
       </c>
       <c r="Q47" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-7.9999999993418669E-6</v>
       </c>
-      <c r="R47" s="1">
-        <f t="shared" si="1"/>
+      <c r="R47" s="6">
+        <f t="shared" si="3"/>
         <v>4.5799999999988211E-6</v>
       </c>
       <c r="T47">
@@ -32938,19 +32972,19 @@
         <v>1.0337571939E-2</v>
       </c>
       <c r="Z47" s="4">
-        <f>F47-W47</f>
+        <f t="shared" si="6"/>
         <v>-1.7224280609990927E-3</v>
       </c>
-      <c r="AA47">
-        <f>E47-X47</f>
+      <c r="AA47" s="5">
+        <f t="shared" si="7"/>
         <v>1.7192280609999999E-3</v>
       </c>
       <c r="AB47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.8187689999999995E-6</v>
       </c>
       <c r="AC47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-8.9446299999986628E-7</v>
       </c>
     </row>
@@ -32964,7 +32998,7 @@
       <c r="D48" s="2">
         <v>8.2700599999999996E-6</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="5">
         <v>1.0337600000000001E-2</v>
       </c>
       <c r="F48" s="4">
@@ -32979,7 +33013,7 @@
       <c r="J48">
         <v>1250</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="5">
         <v>1.033363E-2</v>
       </c>
       <c r="L48">
@@ -32995,11 +33029,11 @@
         <v>8.2669060000000002E-6</v>
       </c>
       <c r="Q48" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-5.999999999062311E-6</v>
       </c>
-      <c r="R48" s="1">
-        <f t="shared" si="1"/>
+      <c r="R48" s="6">
+        <f t="shared" si="3"/>
         <v>3.9700000000007091E-6</v>
       </c>
       <c r="T48">
@@ -33018,19 +33052,19 @@
         <v>8.8634819329999996E-3</v>
       </c>
       <c r="Z48" s="4">
-        <f>F48-W48</f>
+        <f t="shared" si="6"/>
         <v>-1.4765180669993327E-3</v>
       </c>
-      <c r="AA48">
-        <f>E48-X48</f>
+      <c r="AA48" s="5">
+        <f t="shared" si="7"/>
         <v>1.474118067000001E-3</v>
       </c>
       <c r="AB48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.5612519999999994E-6</v>
       </c>
       <c r="AC48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.7098899999971521E-7</v>
       </c>
     </row>
@@ -33044,7 +33078,7 @@
       <c r="D49" s="2">
         <v>7.0907900000000001E-6</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="5">
         <v>8.86348E-3</v>
       </c>
       <c r="F49" s="4">
@@ -33059,7 +33093,7 @@
       <c r="J49">
         <v>1250</v>
       </c>
-      <c r="K49">
+      <c r="K49" s="5">
         <v>8.8601040000000006E-3</v>
       </c>
       <c r="L49">
@@ -33075,11 +33109,11 @@
         <v>7.0880830000000001E-6</v>
       </c>
       <c r="Q49" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R49" s="1">
-        <f t="shared" si="1"/>
+      <c r="R49" s="6">
+        <f t="shared" si="3"/>
         <v>3.3759999999993795E-6</v>
       </c>
       <c r="T49">
@@ -33098,19 +33132,19 @@
         <v>7.5995903529999997E-3</v>
       </c>
       <c r="Z49" s="4">
-        <f>F49-W49</f>
+        <f t="shared" si="6"/>
         <v>-1.2604096470010262E-3</v>
       </c>
-      <c r="AA49">
-        <f>E49-X49</f>
+      <c r="AA49" s="5">
+        <f t="shared" si="7"/>
         <v>1.2638896470000003E-3</v>
       </c>
       <c r="AB49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.4830539999999998E-6</v>
       </c>
       <c r="AC49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-6.5821300000018512E-7</v>
       </c>
     </row>
@@ -33124,7 +33158,7 @@
       <c r="D50" s="2">
         <v>6.07967E-6</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="5">
         <v>7.5995899999999998E-3</v>
       </c>
       <c r="F50" s="4">
@@ -33139,7 +33173,7 @@
       <c r="J50">
         <v>1250</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="5">
         <v>7.5966940000000002E-3</v>
       </c>
       <c r="L50">
@@ -33155,11 +33189,11 @@
         <v>6.0773549999999999E-6</v>
       </c>
       <c r="Q50" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2.9999999995311555E-6</v>
       </c>
-      <c r="R50" s="1">
-        <f t="shared" si="1"/>
+      <c r="R50" s="6">
+        <f t="shared" si="3"/>
         <v>2.895999999999628E-6</v>
       </c>
       <c r="T50">
@@ -33178,19 +33212,19 @@
         <v>6.5159238739999998E-3</v>
       </c>
       <c r="Z50" s="4">
-        <f>F50-W50</f>
+        <f t="shared" si="6"/>
         <v>-1.0840761260002552E-3</v>
       </c>
-      <c r="AA50">
-        <f>E50-X50</f>
+      <c r="AA50" s="5">
+        <f t="shared" si="7"/>
         <v>1.083666126E-3</v>
       </c>
       <c r="AB50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.5585950000000001E-6</v>
       </c>
       <c r="AC50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-5.6172000000020983E-7</v>
       </c>
     </row>
@@ -33204,7 +33238,7 @@
       <c r="D51" s="2">
         <v>5.2127400000000003E-6</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="5">
         <v>6.5159199999999997E-3</v>
       </c>
       <c r="F51" s="4">
@@ -33219,7 +33253,7 @@
       <c r="J51">
         <v>1250</v>
       </c>
-      <c r="K51">
+      <c r="K51" s="5">
         <v>6.5134399999999997E-3</v>
       </c>
       <c r="L51">
@@ -33235,11 +33269,11 @@
         <v>5.2107519999999997E-6</v>
       </c>
       <c r="Q51" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-7.0000000000902673E-6</v>
       </c>
-      <c r="R51" s="1">
-        <f t="shared" si="1"/>
+      <c r="R51" s="6">
+        <f t="shared" si="3"/>
         <v>2.4800000000000169E-6</v>
       </c>
       <c r="T51">
@@ -33258,19 +33292,19 @@
         <v>5.5867832290000001E-3</v>
       </c>
       <c r="Z51" s="4">
-        <f>F51-W51</f>
+        <f t="shared" si="6"/>
         <v>-9.332167709992234E-4</v>
       </c>
-      <c r="AA51">
-        <f>E51-X51</f>
+      <c r="AA51" s="5">
+        <f t="shared" si="7"/>
         <v>9.2913677099999963E-4</v>
       </c>
       <c r="AB51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.7659680000000006E-6</v>
       </c>
       <c r="AC51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-4.8487299999979555E-7</v>
       </c>
     </row>
@@ -33284,7 +33318,7 @@
       <c r="D52" s="2">
         <v>4.4694300000000003E-6</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="5">
         <v>5.5867800000000004E-3</v>
       </c>
       <c r="F52" s="4">
@@ -33299,7 +33333,7 @@
       <c r="J52">
         <v>1250</v>
       </c>
-      <c r="K52">
+      <c r="K52" s="5">
         <v>5.5846539999999997E-3</v>
       </c>
       <c r="L52">
@@ -33315,11 +33349,11 @@
         <v>4.467723E-6</v>
       </c>
       <c r="Q52" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-4.9999999998107114E-6</v>
       </c>
-      <c r="R52" s="1">
-        <f t="shared" si="1"/>
+      <c r="R52" s="6">
+        <f t="shared" si="3"/>
         <v>2.1260000000007315E-6</v>
       </c>
       <c r="T52">
@@ -33338,19 +33372,19 @@
         <v>4.7901337479999999E-3</v>
       </c>
       <c r="Z52" s="4">
-        <f>F52-W52</f>
+        <f t="shared" si="6"/>
         <v>-7.9986625200056949E-4</v>
       </c>
-      <c r="AA52">
-        <f>E52-X52</f>
+      <c r="AA52" s="5">
+        <f t="shared" si="7"/>
         <v>7.9664625200000054E-4</v>
       </c>
       <c r="AB52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.0863650000000005E-6</v>
       </c>
       <c r="AC52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-4.1913000000011469E-7</v>
       </c>
     </row>
@@ -33364,7 +33398,7 @@
       <c r="D53" s="2">
         <v>3.83211E-6</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="5">
         <v>4.7901300000000001E-3</v>
       </c>
       <c r="F53" s="4">
@@ -33379,7 +33413,7 @@
       <c r="J53">
         <v>1250</v>
       </c>
-      <c r="K53">
+      <c r="K53" s="5">
         <v>4.7883079999999998E-3</v>
       </c>
       <c r="L53">
@@ -33395,11 +33429,11 @@
         <v>3.8306460000000002E-6</v>
       </c>
       <c r="Q53" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2.0000000002795559E-6</v>
       </c>
-      <c r="R53" s="1">
-        <f t="shared" si="1"/>
+      <c r="R53" s="6">
+        <f t="shared" si="3"/>
         <v>1.8220000000002817E-6</v>
       </c>
       <c r="T53">
@@ -33418,19 +33452,19 @@
         <v>4.1070828029999996E-3</v>
       </c>
       <c r="Z53" s="4">
-        <f>F53-W53</f>
+        <f t="shared" si="6"/>
         <v>-6.8291719700042108E-4</v>
       </c>
-      <c r="AA53">
-        <f>E53-X53</f>
+      <c r="AA53" s="5">
+        <f t="shared" si="7"/>
         <v>6.8304719700000051E-4</v>
       </c>
       <c r="AB53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.5036689999999998E-6</v>
       </c>
       <c r="AC53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.5431700000018718E-7</v>
       </c>
     </row>
@@ -33444,7 +33478,7 @@
       <c r="D54" s="2">
         <v>3.2856700000000002E-6</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="5">
         <v>4.1070799999999999E-3</v>
       </c>
       <c r="F54" s="4">
@@ -33459,7 +33493,7 @@
       <c r="J54">
         <v>1250</v>
       </c>
-      <c r="K54">
+      <c r="K54" s="5">
         <v>4.1055170000000004E-3</v>
       </c>
       <c r="L54">
@@ -33475,11 +33509,11 @@
         <v>3.2844139999999998E-6</v>
       </c>
       <c r="Q54" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-4.0000000005591119E-6</v>
       </c>
-      <c r="R54" s="1">
-        <f t="shared" si="1"/>
+      <c r="R54" s="6">
+        <f t="shared" si="3"/>
         <v>1.5629999999995647E-6</v>
       </c>
       <c r="T54">
@@ -33498,19 +33532,19 @@
         <v>3.5214317670000002E-3</v>
       </c>
       <c r="Z54" s="4">
-        <f>F54-W54</f>
+        <f t="shared" si="6"/>
         <v>-5.8856823300068584E-4</v>
       </c>
-      <c r="AA54">
-        <f>E54-X54</f>
+      <c r="AA54" s="5">
+        <f t="shared" si="7"/>
         <v>5.8564823299999975E-4</v>
       </c>
       <c r="AB54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.0040630000000002E-6</v>
       </c>
       <c r="AC54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.0885500000056576E-7</v>
       </c>
     </row>

</xml_diff>